<commit_message>
-Changing the Schematic design stile -Correcting some BOM-file data
</commit_message>
<xml_diff>
--- a/HG0B1CEU6N/Released/BOM/HG0B1CEU6N.xlsx
+++ b/HG0B1CEU6N/Released/BOM/HG0B1CEU6N.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HEXABITZ\Projects\STM32-G0-Dip-Module\HG0B1CEU6N\Released\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4482B34C-1785-4E10-9368-F0437C5EB8D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73F32F5-944C-4416-A409-822FAD95537B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23880" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="H21R00" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Manufacturer Part Number</t>
-  </si>
-  <si>
     <t>Manufacturer</t>
   </si>
   <si>
@@ -274,15 +271,6 @@
     <t>R2</t>
   </si>
   <si>
-    <t>CRCW06031R00FKEAHP</t>
-  </si>
-  <si>
-    <t>https://octopart.com/crcw06031r00fkeahp-vishay-46606343?r=sp</t>
-  </si>
-  <si>
-    <t>Res Thick Film 0603 1 Ohm 1% 0.33W(1/3W) ±100ppm/°C</t>
-  </si>
-  <si>
     <t>R3 , R6</t>
   </si>
   <si>
@@ -347,6 +335,18 @@
   </si>
   <si>
     <t>Switch Tactile N.O. SPST Round Button PC Pins 0.05A 12VDC 100000Cycle 1.27N Thru-Hole Bulk</t>
+  </si>
+  <si>
+    <t>'Manufacturer Part Number</t>
+  </si>
+  <si>
+    <t>RCS06031R00FKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 1 OHM 1% 1/4W 0603</t>
+  </si>
+  <si>
+    <t>https://octopart.com/rcs06031r00fkea-vishay-75198106?r=sp</t>
   </si>
 </sst>
 </file>
@@ -556,7 +556,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -573,52 +573,37 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -627,7 +612,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -640,7 +625,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -666,6 +651,12 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1042,506 +1033,490 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A2:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
     <col min="2" max="2" width="70.5703125" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="84" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
     <col min="7" max="7" width="49" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-    </row>
-    <row r="2" spans="1:9" ht="46.5" x14ac:dyDescent="0.7">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="10" t="s">
+    <row r="2" spans="1:7" ht="46.5" x14ac:dyDescent="0.7">
+      <c r="A2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="11"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="28">
+        <v>0</v>
+      </c>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="29">
+        <v>44842</v>
+      </c>
+      <c r="E5" s="30"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="35">
+      <c r="D6" s="32"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="2"/>
+    </row>
+    <row r="8" spans="1:7" s="25" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="36">
-        <v>44842</v>
-      </c>
-      <c r="E5" s="37"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C8" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="F9" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="B12" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="F12" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="24.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="F13" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="F15" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="E16" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="F16" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="39"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="2"/>
-    </row>
-    <row r="8" spans="1:9" s="32" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="30" t="s">
+      <c r="D19" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="16">
         <v>1</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="31" t="s">
+    </row>
+    <row r="20" spans="1:6" ht="24" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="16">
         <v>4</v>
       </c>
-      <c r="D8" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" s="30" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="30" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="21">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="33" t="s">
-        <v>72</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E10" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="22">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E23" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
-        <v>73</v>
-      </c>
-      <c r="B11" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="22">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="B12" s="34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" s="22">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="17" customFormat="1" ht="24.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="B13" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="22">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>81</v>
-      </c>
-      <c r="B14" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="24" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B15" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="E15" s="24" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="22" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>87</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="F16" s="22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E17" s="24" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="B18" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F18" s="22">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="22" t="s">
+      <c r="B27" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C27" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="22" t="s">
-        <v>94</v>
-      </c>
-      <c r="E19" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="F19" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="16" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A20" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="B20" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="F20" s="22">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="B21" s="28" t="s">
-        <v>56</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="24" t="s">
-        <v>29</v>
-      </c>
-      <c r="F21" s="22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="22" t="s">
-        <v>97</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E22" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="24" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="E24" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="F24" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="F25" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="D26" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="24" t="s">
-        <v>53</v>
-      </c>
-      <c r="F26" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="C27" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="22">
+      <c r="F27" s="16">
         <v>1</v>
       </c>
     </row>
@@ -1563,9 +1538,10 @@
     <hyperlink ref="E26" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="E17" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="E11" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E9" r:id="rId12" xr:uid="{53219BB9-545E-4287-81B6-7A59A55F053F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId12"/>
-  <drawing r:id="rId13"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId13"/>
+  <drawing r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>